<commit_message>
some bugs fixed - optional end_date for processing added
</commit_message>
<xml_diff>
--- a/trades.xlsx
+++ b/trades.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t xml:space="preserve">Data do Negócio</t>
   </si>
@@ -41,31 +41,37 @@
     <t xml:space="preserve">Valor</t>
   </si>
   <si>
-    <t xml:space="preserve">06/06/2025</t>
+    <t xml:space="preserve">30/05/2025</t>
   </si>
   <si>
     <t xml:space="preserve">Compra</t>
   </si>
   <si>
+    <t xml:space="preserve">Mercado Fracionário</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XP INVESTIMENTOS CCTVM S/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POSI3F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21/05/2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mercado à Vista</t>
   </si>
   <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
     <t xml:space="preserve">C6 CORRETORA DE TITULOS E VALORES MOBILIARIOS LTDA</t>
   </si>
   <si>
-    <t xml:space="preserve">BBAS3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05/06/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mercado Fracionário</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BBAS3F</t>
+    <t xml:space="preserve">RECV3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20/05/2025</t>
   </si>
 </sst>
 </file>
@@ -146,7 +152,7 @@
     <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="16.6171875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="30.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -198,24 +204,24 @@
         <v>14</v>
       </c>
       <c r="G2" s="5">
-        <v>100</v>
+        <v>17</v>
       </c>
       <c r="H2" s="4">
-        <v>21.75</v>
+        <v>4.72</v>
       </c>
       <c r="I2" s="4">
-        <v>2175</v>
+        <v>80.24</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>12</v>
@@ -224,16 +230,74 @@
         <v>13</v>
       </c>
       <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="5">
+        <v>18</v>
+      </c>
+      <c r="H3" s="4">
+        <v>4.72</v>
+      </c>
+      <c r="I3" s="4">
+        <v>84.96</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="5">
-        <v>50</v>
-      </c>
-      <c r="H3" s="4">
-        <v>22.29</v>
-      </c>
-      <c r="I3" s="4">
-        <v>1114.5</v>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="5">
+        <v>200</v>
+      </c>
+      <c r="H4" s="4">
+        <v>14.27</v>
+      </c>
+      <c r="I4" s="4">
+        <v>2854</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="5">
+        <v>100</v>
+      </c>
+      <c r="H5" s="4">
+        <v>14.03</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1403</v>
       </c>
     </row>
   </sheetData>

</xml_diff>